<commit_message>
Worked on a few bugs
Bugs:
L, O
</commit_message>
<xml_diff>
--- a/Features & Bugs/mixOmics Features & Bugs.xlsx
+++ b/Features & Bugs/mixOmics Features & Bugs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\mixOmics Features &amp; Bugs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\mO Work\Features &amp; Bugs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{480AA883-D53A-4968-B36E-001E451A7DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA7F9EA-3557-4240-9973-B5DC621CA7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1173,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,7 +1308,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="H5" s="5"/>
       <c r="I5" s="2" t="s">
         <v>64</v>
@@ -1316,7 +1316,7 @@
       <c r="J5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="6" t="s">
         <v>66</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -1677,14 +1677,14 @@
         <v>44607</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="6" t="s">
         <v>56</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -1741,7 +1741,7 @@
       <c r="B14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="6" t="s">
         <v>62</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -2410,8 +2410,11 @@
     <hyperlink ref="T14" r:id="rId10" xr:uid="{533FD37A-8803-4F4E-A5A7-BA9EC079997D}"/>
     <hyperlink ref="L12" r:id="rId11" xr:uid="{6B1D8869-C127-4871-8040-5A3A2F1092CB}"/>
     <hyperlink ref="T11" r:id="rId12" xr:uid="{5E6A1031-6346-412E-AC39-2006E1BCE500}"/>
+    <hyperlink ref="K5" r:id="rId13" xr:uid="{60381408-A03E-4997-A3B0-6A7A90977E0E}"/>
+    <hyperlink ref="C13" r:id="rId14" xr:uid="{1CDEA99B-60C9-4162-BEF2-047AF8A8E90D}"/>
+    <hyperlink ref="C14" r:id="rId15" xr:uid="{9938E4A3-07B8-4BC5-B20B-A8468908C3C0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>